<commit_message>
FDB-AOA Weights and Comparison results.
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,19 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\github_profile\DimensionReductionTool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5230BF5C-3188-4F36-A9EE-DB0D8B537E14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCA33E94-39CF-4F7B-8BA6-18E08B571959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scores" sheetId="1" r:id="rId1"/>
+    <sheet name="dimension reduction" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>model</t>
   </si>
@@ -47,13 +61,52 @@
   </si>
   <si>
     <t>fdb_aoa_score</t>
+  </si>
+  <si>
+    <t>Original Data Shape</t>
+  </si>
+  <si>
+    <t>Dimension Reduction (w/ PSO)</t>
+  </si>
+  <si>
+    <t>Dimension Reduction (w/ FDB-AOA)</t>
+  </si>
+  <si>
+    <t>Train</t>
+  </si>
+  <si>
+    <t>(507, 147)</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Extraxted Features</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(168, 147) </t>
+  </si>
+  <si>
+    <t>(507, 130)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(168, 130) </t>
+  </si>
+  <si>
+    <t>(507, 14)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(168, 14) </t>
+  </si>
+  <si>
+    <t>Extracted Feature Rate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -67,6 +120,15 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -105,11 +167,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -417,7 +487,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="G1" sqref="G1:L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -425,6 +495,9 @@
     <col min="2" max="2" width="11.28515625" customWidth="1"/>
     <col min="3" max="3" width="11.85546875" customWidth="1"/>
     <col min="4" max="4" width="16.140625" customWidth="1"/>
+    <col min="7" max="7" width="32.85546875" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" customWidth="1"/>
+    <col min="10" max="10" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -514,4 +587,90 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{227C8DC9-0A97-41AA-8591-44C19C74E7CA}">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3"/>
+      <c r="B1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="2"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3">
+        <v>17</v>
+      </c>
+      <c r="E3" s="5">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4">
+        <f>147-14</f>
+        <v>133</v>
+      </c>
+      <c r="E4" s="5">
+        <v>0.9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>